<commit_message>
Update to api_data. Added ignore prefix.
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="412">
   <si>
     <t>label</t>
   </si>
@@ -1147,27 +1147,15 @@
     <t>denom_uw</t>
   </si>
   <si>
-    <t>implementing_partner</t>
-  </si>
-  <si>
-    <t>primary_donor</t>
-  </si>
-  <si>
     <t>PMA</t>
   </si>
   <si>
     <t>TUL</t>
   </si>
   <si>
-    <t>type_code (for calculating code)</t>
-  </si>
-  <si>
     <t>CORE</t>
   </si>
   <si>
-    <t>survey(_subtype)(_questionnaire)?</t>
-  </si>
-  <si>
     <t>geo_code</t>
   </si>
   <si>
@@ -1186,6 +1174,9 @@
     <t>jef</t>
   </si>
   <si>
+    <t>update</t>
+  </si>
+  <si>
     <t>meta-update</t>
   </si>
   <si>
@@ -1222,9 +1213,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Highlight</t>
-  </si>
-  <si>
     <t>Pink</t>
   </si>
   <si>
@@ -1238,6 +1226,48 @@
   </si>
   <si>
     <t>Insert meaning here.</t>
+  </si>
+  <si>
+    <t>Highlight Rules</t>
+  </si>
+  <si>
+    <t>Column Name Rules</t>
+  </si>
+  <si>
+    <t>Ignore Field Prefix</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Any column/field which starts with a "__" will be ignored and not be read into the database.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>__type_code (for calculating code)</t>
+  </si>
+  <si>
+    <t>__survey(_subtype)(_questionnaire)?</t>
+  </si>
+  <si>
+    <t>__implementing_partner</t>
+  </si>
+  <si>
+    <t>__primary_donor</t>
+  </si>
+  <si>
+    <t>Added Column Name Rule "Ignore Field Prefix" as "__".</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Changed the following fields to be ignored by prefixing with "__": __type_code (for calculating code) __survey(_subtype)(_questionnaire)? __implementing_partner __primary_donor</t>
   </si>
 </sst>
 </file>
@@ -1331,8 +1361,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1629,7 +1671,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="265">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1756,6 +1798,12 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1882,6 +1930,12 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2213,9 +2267,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2224,10 +2278,10 @@
     <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10.5" style="1" bestFit="1" customWidth="1"/>
@@ -2252,16 +2306,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>377</v>
+        <v>406</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>371</v>
+        <v>407</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>372</v>
+        <v>408</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>3</v>
@@ -2296,10 +2350,10 @@
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>373</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="I2" s="4">
         <v>2013</v>
@@ -2563,7 +2617,7 @@
         <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I11" s="4">
         <v>2014</v>
@@ -3470,75 +3524,104 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>390</v>
+      </c>
+      <c r="B1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" t="s">
+        <v>394</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B4" t="s">
+        <v>396</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>398</v>
+      </c>
+      <c r="B5" t="s">
         <v>393</v>
       </c>
-      <c r="B1" t="s">
-        <v>394</v>
-      </c>
-      <c r="C1" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>396</v>
-      </c>
-      <c r="B2" t="s">
-        <v>398</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="C5" s="14" t="s">
+        <v>397</v>
+      </c>
+      <c r="D5" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>399</v>
+      </c>
+      <c r="B6" t="s">
+        <v>400</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>396</v>
-      </c>
-      <c r="B3" t="s">
-        <v>399</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B4" t="s">
-        <v>400</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>396</v>
-      </c>
-      <c r="B5" t="s">
-        <v>397</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>401</v>
+      <c r="D6" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -3554,13 +3637,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3570,22 +3653,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3596,16 +3679,16 @@
         <v>42961</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3616,16 +3699,16 @@
         <v>42961</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3636,16 +3719,16 @@
         <v>42961</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="F4" s="12" t="s">
         <v>384</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>386</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3656,16 +3739,16 @@
         <v>42961</v>
       </c>
       <c r="C5" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>386</v>
-      </c>
       <c r="F5" s="12" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3676,16 +3759,56 @@
         <v>42961</v>
       </c>
       <c r="C6" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>389</v>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>42961</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>381</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
+        <v>42961</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>410</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3705,7 +3828,7 @@
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5259,7 +5382,7 @@
         <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:13">

</xml_diff>

<commit_message>
Updated old field name subgeo_code to geo_code for data_kenya worksheet.
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26340" tabRatio="669" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="411">
   <si>
     <t>label</t>
   </si>
@@ -1136,9 +1136,6 @@
   </si>
   <si>
     <t>char2_code</t>
-  </si>
-  <si>
-    <t>subgeo_code</t>
   </si>
   <si>
     <t>denom_w</t>
@@ -1361,8 +1358,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="265">
+  <cellStyleXfs count="267">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1671,7 +1670,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="265">
+  <cellStyles count="267">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1804,6 +1803,7 @@
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1936,6 +1936,7 @@
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2269,7 +2270,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:H1"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2306,16 +2307,16 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>408</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>3</v>
@@ -2350,10 +2351,10 @@
         <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I2" s="4">
         <v>2013</v>
@@ -2617,7 +2618,7 @@
         <v>75</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I11" s="4">
         <v>2014</v>
@@ -3530,7 +3531,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3542,86 +3543,86 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B1" t="s">
         <v>390</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>391</v>
       </c>
-      <c r="C1" t="s">
-        <v>392</v>
-      </c>
       <c r="D1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>396</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>397</v>
-      </c>
       <c r="D4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>398</v>
+      </c>
+      <c r="B6" t="s">
         <v>399</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>401</v>
-      </c>
       <c r="D6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -3639,11 +3640,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3653,22 +3654,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>375</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>376</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>377</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3679,16 +3680,16 @@
         <v>42961</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3699,16 +3700,16 @@
         <v>42961</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>388</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3719,16 +3720,16 @@
         <v>42961</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>383</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3739,16 +3740,16 @@
         <v>42961</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -3759,16 +3760,16 @@
         <v>42961</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3779,16 +3780,16 @@
         <v>42961</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3799,16 +3800,16 @@
         <v>42961</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>380</v>
-      </c>
       <c r="E8" s="12" t="s">
+        <v>409</v>
+      </c>
+      <c r="F8" s="12" t="s">
         <v>410</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3828,7 +3829,7 @@
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4416,7 +4417,7 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5364,10 +5365,10 @@
         <v>361</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>362</v>
@@ -5382,7 +5383,7 @@
         <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -6090,9 +6091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6136,10 +6137,10 @@
         <v>361</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>369</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>370</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>362</v>
@@ -6154,7 +6155,7 @@
         <v>41</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="2" spans="1:14">

</xml_diff>

<commit_message>
Changed code to pull from Postgres rather than SqlLite.
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -1496,7 +1496,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1506,6 +1506,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="239">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3558,8 +3559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3572,7 +3573,8 @@
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="32.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="9"/>
+    <col min="12" max="12" width="13.1640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3606,10 +3608,10 @@
       <c r="J1" t="s">
         <v>320</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="9" t="s">
         <v>322</v>
       </c>
     </row>
@@ -3644,10 +3646,10 @@
       <c r="J2" t="s">
         <v>337</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="9">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="9">
         <v>1</v>
       </c>
     </row>
@@ -3714,10 +3716,10 @@
       <c r="J4" t="s">
         <v>337</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="9">
         <v>1</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="9">
         <v>2</v>
       </c>
     </row>
@@ -4042,7 +4044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update models for datalab init. Update source data.
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="26280" tabRatio="669" activeTab="3"/>
+    <workbookView xWindow="16520" yWindow="7920" windowWidth="24560" windowHeight="18300" tabRatio="669" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="387">
   <si>
     <t>label</t>
   </si>
@@ -1145,9 +1145,6 @@
     <t>CORE</t>
   </si>
   <si>
-    <t>geo_code</t>
-  </si>
-  <si>
     <t>__type_code (for calculating code)</t>
   </si>
   <si>
@@ -1170,6 +1167,27 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>subheading</t>
+  </si>
+  <si>
+    <t>gh_national</t>
+  </si>
+  <si>
+    <t>ke_national</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>Household / female questionnaire</t>
   </si>
 </sst>
 </file>
@@ -1255,8 +1273,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="239">
+  <cellStyleXfs count="257">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1508,7 +1544,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="239">
+  <cellStyles count="257">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1628,6 +1664,15 @@
     <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1747,6 +1792,15 @@
     <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2079,11 +2133,12 @@
   <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.83203125" style="6" customWidth="1"/>
@@ -2107,16 +2162,16 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>375</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>376</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
@@ -2144,6 +2199,10 @@
       </c>
     </row>
     <row r="2" spans="1:15">
+      <c r="A2" t="str">
+        <f t="shared" ref="A2:A41" si="0">H2&amp;" Round "&amp;I2</f>
+        <v>2013 Round 1</v>
+      </c>
       <c r="B2">
         <v>101</v>
       </c>
@@ -2177,8 +2236,15 @@
       <c r="N2" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="O2" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="3" spans="1:15">
+      <c r="A3" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 2</v>
+      </c>
       <c r="B3">
         <v>102</v>
       </c>
@@ -2206,8 +2272,15 @@
       <c r="N3" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="O3" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="4" spans="1:15">
+      <c r="A4" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 3</v>
+      </c>
       <c r="B4">
         <v>103</v>
       </c>
@@ -2235,8 +2308,15 @@
       <c r="N4" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="O4" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="5" spans="1:15">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 4</v>
+      </c>
       <c r="B5">
         <v>104</v>
       </c>
@@ -2264,8 +2344,15 @@
       <c r="N5" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="O5" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="6" spans="1:15">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 5</v>
+      </c>
       <c r="B6">
         <v>105</v>
       </c>
@@ -2293,8 +2380,15 @@
       <c r="N6" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="O6" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="7" spans="1:15">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 1</v>
+      </c>
       <c r="B7">
         <v>201</v>
       </c>
@@ -2324,6 +2418,10 @@
       </c>
     </row>
     <row r="8" spans="1:15">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 2</v>
+      </c>
       <c r="B8">
         <v>202</v>
       </c>
@@ -2353,6 +2451,10 @@
       </c>
     </row>
     <row r="9" spans="1:15">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 3</v>
+      </c>
       <c r="B9">
         <v>203</v>
       </c>
@@ -2382,6 +2484,10 @@
       </c>
     </row>
     <row r="10" spans="1:15">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 4</v>
+      </c>
       <c r="B10">
         <v>204</v>
       </c>
@@ -2411,6 +2517,10 @@
       </c>
     </row>
     <row r="11" spans="1:15">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 1</v>
+      </c>
       <c r="B11">
         <v>301</v>
       </c>
@@ -2443,6 +2553,10 @@
       </c>
     </row>
     <row r="12" spans="1:15">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 2</v>
+      </c>
       <c r="B12">
         <v>302</v>
       </c>
@@ -2472,6 +2586,10 @@
       </c>
     </row>
     <row r="13" spans="1:15">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 3</v>
+      </c>
       <c r="B13">
         <v>303</v>
       </c>
@@ -2501,6 +2619,10 @@
       </c>
     </row>
     <row r="14" spans="1:15">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 4</v>
+      </c>
       <c r="B14">
         <v>304</v>
       </c>
@@ -2530,6 +2652,10 @@
       </c>
     </row>
     <row r="15" spans="1:15">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 5</v>
+      </c>
       <c r="B15">
         <v>305</v>
       </c>
@@ -2559,6 +2685,10 @@
       </c>
     </row>
     <row r="16" spans="1:15">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 1</v>
+      </c>
       <c r="B16">
         <v>401</v>
       </c>
@@ -2587,7 +2717,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="1:15">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 2</v>
+      </c>
       <c r="B17">
         <v>402</v>
       </c>
@@ -2616,7 +2750,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="2:14">
+    <row r="18" spans="1:15">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 3</v>
+      </c>
       <c r="B18">
         <v>403</v>
       </c>
@@ -2645,7 +2783,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="2:14">
+    <row r="19" spans="1:15">
+      <c r="A19" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 1</v>
+      </c>
       <c r="B19">
         <v>501</v>
       </c>
@@ -2674,7 +2816,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:14">
+    <row r="20" spans="1:15">
+      <c r="A20" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 2</v>
+      </c>
       <c r="B20">
         <v>502</v>
       </c>
@@ -2703,7 +2849,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="1:15">
+      <c r="A21" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 3</v>
+      </c>
       <c r="B21">
         <v>503</v>
       </c>
@@ -2732,7 +2882,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:14">
+    <row r="22" spans="1:15">
+      <c r="A22" t="str">
+        <f t="shared" si="0"/>
+        <v>2017 Round 4</v>
+      </c>
       <c r="B22">
         <v>504</v>
       </c>
@@ -2761,7 +2915,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="1:15">
+      <c r="A23" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 1</v>
+      </c>
       <c r="B23">
         <v>601</v>
       </c>
@@ -2789,8 +2947,15 @@
       <c r="N23" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="24" spans="2:14">
+      <c r="O23" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 2</v>
+      </c>
       <c r="B24">
         <v>602</v>
       </c>
@@ -2818,8 +2983,15 @@
       <c r="N24" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="2:14">
+      <c r="O24" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 3</v>
+      </c>
       <c r="B25">
         <v>603</v>
       </c>
@@ -2847,8 +3019,15 @@
       <c r="N25" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="2:14">
+      <c r="O25" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 4</v>
+      </c>
       <c r="B26">
         <v>604</v>
       </c>
@@ -2876,8 +3055,15 @@
       <c r="N26" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="2:14">
+      <c r="O26" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" t="str">
+        <f t="shared" si="0"/>
+        <v>2017 Round 5</v>
+      </c>
       <c r="B27">
         <v>605</v>
       </c>
@@ -2905,8 +3091,15 @@
       <c r="N27" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="2:14">
+      <c r="O27" s="7" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 1</v>
+      </c>
       <c r="B28">
         <v>701</v>
       </c>
@@ -2935,7 +3128,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="2:14">
+    <row r="29" spans="1:15">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 2</v>
+      </c>
       <c r="B29">
         <v>702</v>
       </c>
@@ -2964,7 +3161,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="2:14">
+    <row r="30" spans="1:15">
+      <c r="A30" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 3</v>
+      </c>
       <c r="B30">
         <v>703</v>
       </c>
@@ -2993,7 +3194,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="2:14">
+    <row r="31" spans="1:15">
+      <c r="A31" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 4</v>
+      </c>
       <c r="B31">
         <v>704</v>
       </c>
@@ -3022,7 +3227,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:14">
+    <row r="32" spans="1:15">
+      <c r="A32" t="str">
+        <f t="shared" si="0"/>
+        <v>2017 Round 5</v>
+      </c>
       <c r="B32">
         <v>705</v>
       </c>
@@ -3051,7 +3260,11 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:14">
+    <row r="33" spans="1:14">
+      <c r="A33" t="str">
+        <f t="shared" si="0"/>
+        <v>2014 Round 1</v>
+      </c>
       <c r="B33">
         <v>801</v>
       </c>
@@ -3080,7 +3293,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:14">
+    <row r="34" spans="1:14">
+      <c r="A34" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 2</v>
+      </c>
       <c r="B34">
         <v>802</v>
       </c>
@@ -3109,7 +3326,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="2:14">
+    <row r="35" spans="1:14">
+      <c r="A35" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 3</v>
+      </c>
       <c r="B35">
         <v>803</v>
       </c>
@@ -3138,7 +3359,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:14">
+    <row r="36" spans="1:14">
+      <c r="A36" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 4</v>
+      </c>
       <c r="B36">
         <v>804</v>
       </c>
@@ -3167,7 +3392,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="2:14">
+    <row r="37" spans="1:14">
+      <c r="A37" t="str">
+        <f t="shared" si="0"/>
+        <v>2017 Round 5</v>
+      </c>
       <c r="B37">
         <v>805</v>
       </c>
@@ -3196,7 +3425,11 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="2:14">
+    <row r="38" spans="1:14">
+      <c r="A38" t="str">
+        <f t="shared" si="0"/>
+        <v>2015 Round 1</v>
+      </c>
       <c r="B38">
         <v>901</v>
       </c>
@@ -3225,7 +3458,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="2:14">
+    <row r="39" spans="1:14">
+      <c r="A39" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 2</v>
+      </c>
       <c r="B39">
         <v>902</v>
       </c>
@@ -3254,7 +3491,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="2:14">
+    <row r="40" spans="1:14">
+      <c r="A40" t="str">
+        <f t="shared" si="0"/>
+        <v>2016 Round 1</v>
+      </c>
       <c r="B40">
         <v>1001</v>
       </c>
@@ -3283,7 +3524,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:14">
+    <row r="41" spans="1:14">
+      <c r="A41" t="str">
+        <f t="shared" si="0"/>
+        <v>2017 Round 2</v>
+      </c>
       <c r="B41">
         <v>1002</v>
       </c>
@@ -3328,7 +3573,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3559,7 +3804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3896,19 +4141,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>199</v>
       </c>
@@ -3918,19 +4164,31 @@
       <c r="C1" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" t="s">
         <v>377</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>378</v>
       </c>
-      <c r="C2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>213</v>
       </c>
@@ -3940,8 +4198,14 @@
       <c r="C3" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1">
+        <v>101</v>
+      </c>
+      <c r="E3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>203</v>
       </c>
@@ -3951,8 +4215,14 @@
       <c r="C4" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1">
+        <v>102</v>
+      </c>
+      <c r="E4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>204</v>
       </c>
@@ -3962,8 +4232,14 @@
       <c r="C5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>205</v>
       </c>
@@ -3973,8 +4249,14 @@
       <c r="C6" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>206</v>
       </c>
@@ -3984,8 +4266,14 @@
       <c r="C7" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1">
+        <v>105</v>
+      </c>
+      <c r="E7" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -3995,8 +4283,14 @@
       <c r="C8" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -4006,8 +4300,14 @@
       <c r="C9" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>284</v>
       </c>
@@ -4017,8 +4317,14 @@
       <c r="C10" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1">
+        <v>106</v>
+      </c>
+      <c r="E10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>285</v>
       </c>
@@ -4027,6 +4333,12 @@
       </c>
       <c r="C11" t="s">
         <v>305</v>
+      </c>
+      <c r="D11" s="1">
+        <v>107</v>
+      </c>
+      <c r="E11" t="s">
+        <v>386</v>
       </c>
     </row>
   </sheetData>
@@ -4071,13 +4383,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -4796,18 +5108,59 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>382</v>
+      </c>
+      <c r="C2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>383</v>
+      </c>
+      <c r="C3" t="s">
+        <v>384</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -4820,10 +5173,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4833,10 +5186,9 @@
     <col min="9" max="9" width="13.5" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.83203125" style="7" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>355</v>
       </c>
@@ -4873,11 +5225,8 @@
       <c r="L1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>15.4</v>
       </c>
@@ -4891,13 +5240,13 @@
         <v>338</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>14.1</v>
       </c>
@@ -4914,7 +5263,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>16.8</v>
       </c>
@@ -4931,7 +5280,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>14.3</v>
       </c>
@@ -4948,7 +5297,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>14.7</v>
       </c>
@@ -4965,7 +5314,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>15.6</v>
       </c>
@@ -4982,7 +5331,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>16.2</v>
       </c>
@@ -4996,7 +5345,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>14.3</v>
       </c>
@@ -5010,7 +5359,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>16.100000000000001</v>
       </c>
@@ -5021,13 +5370,13 @@
         <v>338</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L10" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>14.6</v>
       </c>
@@ -5041,7 +5390,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>17.7</v>
       </c>
@@ -5055,7 +5404,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>15.6</v>
       </c>
@@ -5069,7 +5418,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>14.7</v>
       </c>
@@ -5083,7 +5432,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>15.2</v>
       </c>
@@ -5097,7 +5446,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>19.899999999999999</v>
       </c>
@@ -5136,7 +5485,7 @@
         <v>338</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L18" s="7" t="s">
         <v>41</v>
@@ -5251,7 +5600,7 @@
         <v>342</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>47</v>
@@ -5366,7 +5715,7 @@
         <v>342</v>
       </c>
       <c r="J34" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>42</v>
@@ -5481,7 +5830,7 @@
         <v>342</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L42" s="7" t="s">
         <v>41</v>
@@ -5598,10 +5947,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5618,10 +5967,9 @@
     <col min="10" max="10" width="13.5" style="7" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>199</v>
       </c>
@@ -5661,11 +6009,8 @@
       <c r="M1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:13">
       <c r="B2">
         <v>41.8</v>
       </c>
@@ -5676,13 +6021,13 @@
         <v>338</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M2" s="7" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="B3">
         <v>43.8</v>
       </c>
@@ -5696,7 +6041,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="B4">
         <v>40.200000000000003</v>
       </c>
@@ -5710,7 +6055,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="B5">
         <v>37.6</v>
       </c>
@@ -5724,7 +6069,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="B6">
         <v>44.4</v>
       </c>
@@ -5738,7 +6083,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="B7">
         <v>44</v>
       </c>
@@ -5752,7 +6097,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="B8">
         <v>42.8</v>
       </c>
@@ -5766,7 +6111,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="B9">
         <v>42.9</v>
       </c>
@@ -5780,7 +6125,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:13">
       <c r="B10">
         <v>40.9</v>
       </c>
@@ -5791,13 +6136,13 @@
         <v>338</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:13">
       <c r="B11">
         <v>44.2</v>
       </c>
@@ -5811,7 +6156,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:13">
       <c r="B12">
         <v>38.799999999999997</v>
       </c>
@@ -5825,7 +6170,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:13">
       <c r="B13">
         <v>39.700000000000003</v>
       </c>
@@ -5839,7 +6184,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:13">
       <c r="B14">
         <v>38.5</v>
       </c>
@@ -5853,7 +6198,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:13">
       <c r="B15">
         <v>40.700000000000003</v>
       </c>
@@ -5867,7 +6212,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:13">
       <c r="B16">
         <v>42.6</v>
       </c>
@@ -5906,7 +6251,7 @@
         <v>338</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>362</v>
@@ -6021,7 +6366,7 @@
         <v>342</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>130</v>
@@ -6136,7 +6481,7 @@
         <v>342</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M34" s="7" t="s">
         <v>133</v>
@@ -6251,7 +6596,7 @@
         <v>342</v>
       </c>
       <c r="K42" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M42" s="7" t="s">
         <v>362</v>

</xml_diff>

<commit_message>
Made update to UI strings.
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="7920" windowWidth="24560" windowHeight="18300" tabRatio="669" activeTab="8"/>
+    <workbookView xWindow="16520" yWindow="7920" windowWidth="24560" windowHeight="18300" tabRatio="669" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="390">
   <si>
     <t>label</t>
   </si>
@@ -1188,6 +1188,15 @@
   </si>
   <si>
     <t>Household / female questionnaire</t>
+  </si>
+  <si>
+    <t>__english</t>
+  </si>
+  <si>
+    <t>__language</t>
+  </si>
+  <si>
+    <t>__value</t>
   </si>
 </sst>
 </file>
@@ -3785,12 +3794,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>387</v>
+      </c>
+      <c r="B1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5949,9 +5972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>

</xml_diff>

<commit_message>
Add partner data to survey and datalab/init
</commit_message>
<xml_diff>
--- a/data/api_data.xlsx
+++ b/data/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="7920" windowWidth="24560" windowHeight="18300" tabRatio="669" activeTab="8"/>
+    <workbookView xWindow="6500" yWindow="2700" windowWidth="24560" windowHeight="18300" tabRatio="669"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="398">
   <si>
     <t>label</t>
   </si>
@@ -1188,13 +1188,46 @@
   </si>
   <si>
     <t>Household / female questionnaire</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>Kwame Nkruma University of Science and Technology (KNUST)</t>
+  </si>
+  <si>
+    <t>Burkina Faso National Institute of Statistics and Demography</t>
+  </si>
+  <si>
+    <t>Tulane University School of Public Health, University of Kinshasa School of Public Health</t>
+  </si>
+  <si>
+    <t>Niger/Niamey National Institute of Statistics</t>
+  </si>
+  <si>
+    <t>Centre for Research, Evaluation Resources and Development (CRERD), Bayero University Kano (BUK)</t>
+  </si>
+  <si>
+    <t>International Centre for Reproductive Health Kenya (ICRHK)</t>
+  </si>
+  <si>
+    <t>School of Public Health, College of Health Sciences, Makerere University in Kampala</t>
+  </si>
+  <si>
+    <t>Addis Ababa University, School of Public Health</t>
+  </si>
+  <si>
+    <t>National Population and Family Planning Board of Indonesia (BkkbN), Universitas Gadjah Mada (UGM), Universitas Hasanuddin (UNHAS), Universitas Sumatera Utara (USU)</t>
+  </si>
+  <si>
+    <t>IIHMR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1224,6 +1257,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1273,7 +1311,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="257">
+  <cellStyleXfs count="261">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1531,8 +1569,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1543,8 +1585,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="257">
+  <cellStyles count="261">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1673,6 +1716,8 @@
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1801,6 +1846,8 @@
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2130,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="H13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="P42" sqref="P42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2151,7 +2198,7 @@
     <col min="15" max="15" width="14.83203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2197,8 +2244,11 @@
       <c r="O1" s="7" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A41" si="0">H2&amp;" Round "&amp;I2</f>
         <v>2013 Round 1</v>
@@ -2239,8 +2289,11 @@
       <c r="O2" s="7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 2</v>
@@ -2275,8 +2328,11 @@
       <c r="O3" s="7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 3</v>
@@ -2311,8 +2367,11 @@
       <c r="O4" s="7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 4</v>
@@ -2347,8 +2406,11 @@
       <c r="O5" s="7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 5</v>
@@ -2383,8 +2445,11 @@
       <c r="O6" s="7" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" s="10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 1</v>
@@ -2416,8 +2481,11 @@
       <c r="N7" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 2</v>
@@ -2449,8 +2517,11 @@
       <c r="N8" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 3</v>
@@ -2482,8 +2553,11 @@
       <c r="N9" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 4</v>
@@ -2515,8 +2589,11 @@
       <c r="N10" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 1</v>
@@ -2551,8 +2628,11 @@
       <c r="N11" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 2</v>
@@ -2584,8 +2664,11 @@
       <c r="N12" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:15">
+      <c r="P12" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 3</v>
@@ -2617,8 +2700,11 @@
       <c r="N13" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:15">
+      <c r="P13" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 4</v>
@@ -2650,8 +2736,11 @@
       <c r="N14" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:15">
+      <c r="P14" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 5</v>
@@ -2683,8 +2772,11 @@
       <c r="N15" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:15">
+      <c r="P15" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 1</v>
@@ -2716,8 +2808,11 @@
       <c r="N16" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="P16" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 2</v>
@@ -2749,8 +2844,11 @@
       <c r="N17" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:15">
+      <c r="P17" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 3</v>
@@ -2782,8 +2880,11 @@
       <c r="N18" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:15">
+      <c r="P18" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 1</v>
@@ -2815,8 +2916,11 @@
       <c r="N19" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:15">
+      <c r="P19" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 2</v>
@@ -2848,8 +2952,11 @@
       <c r="N20" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="1:15">
+      <c r="P20" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 3</v>
@@ -2881,8 +2988,11 @@
       <c r="N21" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:15">
+      <c r="P21" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
         <v>2017 Round 4</v>
@@ -2914,8 +3024,11 @@
       <c r="N22" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:15">
+      <c r="P22" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 1</v>
@@ -2950,8 +3063,11 @@
       <c r="O23" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="P23" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 2</v>
@@ -2986,8 +3102,11 @@
       <c r="O24" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="P24" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 3</v>
@@ -3022,8 +3141,11 @@
       <c r="O25" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="P25" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 4</v>
@@ -3058,8 +3180,11 @@
       <c r="O26" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="P26" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
         <v>2017 Round 5</v>
@@ -3094,8 +3219,11 @@
       <c r="O27" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="P27" s="1" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 1</v>
@@ -3127,8 +3255,11 @@
       <c r="N28" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="P28" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 2</v>
@@ -3160,8 +3291,11 @@
       <c r="N29" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 3</v>
@@ -3193,8 +3327,11 @@
       <c r="N30" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 4</v>
@@ -3226,8 +3363,11 @@
       <c r="N31" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="str">
         <f t="shared" si="0"/>
         <v>2017 Round 5</v>
@@ -3259,8 +3399,11 @@
       <c r="N32" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:14">
+      <c r="P32" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="str">
         <f t="shared" si="0"/>
         <v>2014 Round 1</v>
@@ -3292,8 +3435,11 @@
       <c r="N33" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="1:14">
+      <c r="P33" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 2</v>
@@ -3325,8 +3471,11 @@
       <c r="N34" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:14">
+      <c r="P34" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 3</v>
@@ -3358,8 +3507,11 @@
       <c r="N35" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:14">
+      <c r="P35" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 4</v>
@@ -3391,8 +3543,11 @@
       <c r="N36" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:14">
+      <c r="P36" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="str">
         <f t="shared" si="0"/>
         <v>2017 Round 5</v>
@@ -3424,8 +3579,11 @@
       <c r="N37" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="38" spans="1:14">
+      <c r="P37" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="str">
         <f t="shared" si="0"/>
         <v>2015 Round 1</v>
@@ -3457,8 +3615,11 @@
       <c r="N38" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="39" spans="1:14">
+      <c r="P38" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 2</v>
@@ -3490,8 +3651,11 @@
       <c r="N39" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="40" spans="1:14">
+      <c r="P39" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="str">
         <f t="shared" si="0"/>
         <v>2016 Round 1</v>
@@ -3523,8 +3687,11 @@
       <c r="N40" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="41" spans="1:14">
+      <c r="P40" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="str">
         <f t="shared" si="0"/>
         <v>2017 Round 2</v>
@@ -3555,6 +3722,9 @@
       </c>
       <c r="N41" s="7" t="s">
         <v>27</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>
@@ -5949,7 +6119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>